<commit_message>
Excel Template: Renaming of columns from “Then_Question” to “Then_Goto” and from “Else_Question”  to “Else_Goto”
</commit_message>
<xml_diff>
--- a/Epi Info Web Survey/Epi.Web/Content/Text/Survey.xlsx
+++ b/Epi Info Web Survey/Epi.Web/Content/Text/Survey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vwm5\Source\Repos\MyRepo\EIWSSandbox\Epi.Web\Content\Text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDC\Workspace\Epi Info Web Survey\Epi.Web\Content\Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -106,12 +106,6 @@
     <t>pregnant</t>
   </si>
   <si>
-    <t>Then_Question</t>
-  </si>
-  <si>
-    <t>Else_Question</t>
-  </si>
-  <si>
     <t>When did symptoms start?</t>
   </si>
   <si>
@@ -152,6 +146,12 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>Then_Goto</t>
+  </si>
+  <si>
+    <t>Else_Goto</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,10 +501,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -522,10 +522,10 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -553,10 +553,10 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -576,7 +576,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -597,7 +597,7 @@
         <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -605,10 +605,10 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -622,19 +622,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>